<commit_message>
Update jurnal & templates
</commit_message>
<xml_diff>
--- a/jurnals/list-jurnals.xlsx
+++ b/jurnals/list-jurnals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\project-skripsi\jurnals\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3048F4B-2638-4FB0-8A8B-459401C62C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28789E1C-18CB-48E0-94FF-2079675FB448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1080" yWindow="1080" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SUMBER" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="19">
   <si>
     <t>NO</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Testing React Applications Using React Testing Librar</t>
+  </si>
+  <si>
+    <t>PENERJEMAH BAHASA ALAMI DALAM BAHASA INDONESIA KE SOURCE CODE DALAM BAHASA PASCAL</t>
   </si>
 </sst>
 </file>
@@ -310,6 +313,21 @@
   </cellStyles>
   <dxfs count="10">
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -321,21 +339,6 @@
           <color indexed="64"/>
         </top>
         <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -442,8 +445,8 @@
     <tableColumn id="1" xr3:uid="{2AA735FC-47C5-4130-AEB2-693402EB0B9F}" name="NO" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{BC9F046A-C1EE-4AEC-8B89-7C5365FAF37A}" name="JUDUL" dataDxfId="3"/>
     <tableColumn id="7" xr3:uid="{30C2C0B9-AC83-440E-BEE5-9356B0E7FAE7}" name="TANGGAL" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{956132F0-1847-4697-94B9-48155A15F61D}" name="OFFLINE" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{6995AE5E-DA65-478E-91B6-C191509C8F29}" name="ONLINE" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{956132F0-1847-4697-94B9-48155A15F61D}" name="OFFLINE" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{6995AE5E-DA65-478E-91B6-C191509C8F29}" name="ONLINE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -715,7 +718,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,10 +939,18 @@
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="8"/>
+      <c r="B13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="15">
+        <v>45273</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
@@ -1033,11 +1044,13 @@
     <hyperlink ref="E11" r:id="rId16" xr:uid="{01C0260D-5F29-4148-BC8C-FAD52A5B91CF}"/>
     <hyperlink ref="E12" r:id="rId17" xr:uid="{4D228136-C3C2-4EEC-B026-45389D0F0A84}"/>
     <hyperlink ref="D12" r:id="rId18" xr:uid="{BCFE30C8-1529-47C3-9F1E-D57AB3625FC1}"/>
+    <hyperlink ref="D13" r:id="rId19" xr:uid="{1CCADC27-FF2C-4140-8EF4-A8606812A987}"/>
+    <hyperlink ref="E13" r:id="rId20" xr:uid="{2C2F50F6-E9AF-4D87-996F-68F376557488}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
   <tableParts count="1">
-    <tablePart r:id="rId20"/>
+    <tablePart r:id="rId22"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>